<commit_message>
time management 10.12 edit
</commit_message>
<xml_diff>
--- a/doc/time_management.xlsx
+++ b/doc/time_management.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lian Studer\Documents\Projects\gitty\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347D9DC2-4EB5-41F2-9B32-4CB717DAFA2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC459DD-30B2-46E4-AD5B-0306E4B980BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1606,10 +1606,10 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>11</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9.5</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2114,7 +2114,7 @@
   <dimension ref="A1:BJ42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+      <selection activeCell="Q42" sqref="Q42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3394,7 +3394,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D29)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3623,7 +3623,7 @@
       </c>
       <c r="D21" s="80">
         <f t="shared" si="0"/>
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52"/>
@@ -3638,7 +3638,7 @@
       <c r="O21" s="60"/>
       <c r="P21" s="55"/>
       <c r="Q21" s="63">
-        <v>2</v>
+        <v>2.5</v>
       </c>
       <c r="R21" s="56"/>
       <c r="S21" s="57"/>
@@ -3698,7 +3698,7 @@
       </c>
       <c r="D22" s="80">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3713,7 +3713,7 @@
       <c r="O22" s="60"/>
       <c r="P22" s="55"/>
       <c r="Q22" s="63">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="R22" s="56"/>
       <c r="S22" s="57"/>
@@ -4281,7 +4281,7 @@
       </c>
       <c r="D30" s="42">
         <f>SUM(D31:D34)</f>
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="31"/>
@@ -4500,7 +4500,7 @@
       </c>
       <c r="D33" s="80">
         <f t="shared" si="1"/>
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="E33" s="50"/>
       <c r="F33" s="51"/>
@@ -4514,7 +4514,7 @@
       <c r="N33" s="59"/>
       <c r="O33" s="60"/>
       <c r="P33" s="63">
-        <v>6.5</v>
+        <v>6</v>
       </c>
       <c r="Q33" s="55">
         <v>3</v>
@@ -5154,7 +5154,7 @@
       </c>
       <c r="D42" s="37">
         <f>D38+D35+D30+D18+D14+D9</f>
-        <v>27.25</v>
+        <v>27.75</v>
       </c>
       <c r="E42" s="37"/>
       <c r="F42" s="38"/>
@@ -5196,11 +5196,11 @@
       </c>
       <c r="P42" s="39">
         <f t="shared" si="3"/>
-        <v>9</v>
+        <v>8.5</v>
       </c>
       <c r="Q42" s="39">
         <f t="shared" si="3"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="R42" s="39">
         <f t="shared" si="3"/>
@@ -5486,7 +5486,7 @@
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>
@@ -5503,7 +5503,7 @@
       </c>
       <c r="D6" s="77">
         <f>Zeitplanung!D30</f>
-        <v>9.5</v>
+        <v>9</v>
       </c>
       <c r="F6" s="78"/>
     </row>

</xml_diff>

<commit_message>
update time mgmt 11.12
</commit_message>
<xml_diff>
--- a/doc/time_management.xlsx
+++ b/doc/time_management.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lian Studer\Documents\Projects\gitty\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EC459DD-30B2-46E4-AD5B-0306E4B980BF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0746ED88-F579-413B-A200-376BFAF35DDE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1606,10 +1606,10 @@
                   <c:v>4.5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>9</c:v>
+                  <c:v>11</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -2113,8 +2113,8 @@
   </sheetPr>
   <dimension ref="A1:BJ42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="160" zoomScaleNormal="160" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -2966,7 +2966,9 @@
       <c r="O12" s="60"/>
       <c r="P12" s="61"/>
       <c r="Q12" s="61"/>
-      <c r="R12" s="63"/>
+      <c r="R12" s="63">
+        <v>0</v>
+      </c>
       <c r="S12" s="57"/>
       <c r="T12" s="58"/>
       <c r="U12" s="59"/>
@@ -3394,7 +3396,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D29)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3623,7 +3625,7 @@
       </c>
       <c r="D21" s="80">
         <f t="shared" si="0"/>
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="E21" s="50"/>
       <c r="F21" s="52"/>
@@ -3640,7 +3642,9 @@
       <c r="Q21" s="63">
         <v>2.5</v>
       </c>
-      <c r="R21" s="56"/>
+      <c r="R21" s="56">
+        <v>2</v>
+      </c>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
       <c r="U21" s="59"/>
@@ -3698,7 +3702,7 @@
       </c>
       <c r="D22" s="80">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>4.5</v>
       </c>
       <c r="E22" s="50"/>
       <c r="F22" s="51"/>
@@ -3715,7 +3719,9 @@
       <c r="Q22" s="63">
         <v>0.5</v>
       </c>
-      <c r="R22" s="56"/>
+      <c r="R22" s="56">
+        <v>4</v>
+      </c>
       <c r="S22" s="57"/>
       <c r="T22" s="58"/>
       <c r="U22" s="59"/>
@@ -3788,7 +3794,9 @@
       <c r="O23" s="60"/>
       <c r="P23" s="55"/>
       <c r="Q23" s="55"/>
-      <c r="R23" s="63"/>
+      <c r="R23" s="63">
+        <v>0</v>
+      </c>
       <c r="S23" s="57"/>
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
@@ -4281,7 +4289,7 @@
       </c>
       <c r="D30" s="42">
         <f>SUM(D31:D34)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E30" s="32"/>
       <c r="F30" s="31"/>
@@ -4500,7 +4508,7 @@
       </c>
       <c r="D33" s="80">
         <f t="shared" si="1"/>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="E33" s="50"/>
       <c r="F33" s="51"/>
@@ -4519,7 +4527,9 @@
       <c r="Q33" s="55">
         <v>3</v>
       </c>
-      <c r="R33" s="63"/>
+      <c r="R33" s="63">
+        <v>2</v>
+      </c>
       <c r="S33" s="57"/>
       <c r="T33" s="58"/>
       <c r="U33" s="59"/>
@@ -5154,7 +5164,7 @@
       </c>
       <c r="D42" s="37">
         <f>D38+D35+D30+D18+D14+D9</f>
-        <v>27.75</v>
+        <v>35.75</v>
       </c>
       <c r="E42" s="37"/>
       <c r="F42" s="38"/>
@@ -5204,7 +5214,7 @@
       </c>
       <c r="R42" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="S42" s="39">
         <f t="shared" si="3"/>
@@ -5486,7 +5496,7 @@
       </c>
       <c r="D5" s="77">
         <f>Zeitplanung!D18</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="E5" s="79"/>
       <c r="F5" s="78"/>
@@ -5503,7 +5513,7 @@
       </c>
       <c r="D6" s="77">
         <f>Zeitplanung!D30</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="F6" s="78"/>
     </row>

</xml_diff>